<commit_message>
Mejora deteccion en Skyway, deteccion de fechas cambiada en Thyssenkrupp Campo Limpo y Thyssenkrupp Crankshaft, calculo de resultados
</commit_message>
<xml_diff>
--- a/AI_Engine/Config/formats.xlsx
+++ b/AI_Engine/Config/formats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proyectos\Nueva carpeta\Bot-Creacion-de-Pedidos\AI_Engine\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005AA1C1-20EB-4DFC-80DA-0672583A7D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670F138C-D8E8-471A-89EA-64FF047E1F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{CB7259FD-4C9D-4A4E-AB12-F728DAD994BD}"/>
+    <workbookView xWindow="-130" yWindow="10690" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{CB7259FD-4C9D-4A4E-AB12-F728DAD994BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -511,10 +511,10 @@
     <t>D 31.12.2012</t>
   </si>
   <si>
-    <t>[a-zA-Z]+\d{4,}+</t>
-  </si>
-  <si>
-    <t>[a-zA-Z]*\d{5,}+</t>
+    <t>[a-zA-Z]+\d{4,}</t>
+  </si>
+  <si>
+    <t>[a-zA-Z]*\d{5,}</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1711,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA94B6A-80FD-4C88-8BB5-B4942723B82A}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2362,7 +2362,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2423,12 +2423,13 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2437,7 +2438,7 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2455,12 +2456,13 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2469,7 +2471,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>136</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambiado formato D dd.mm.yyy
</commit_message>
<xml_diff>
--- a/AI_Engine/Config/formats.xlsx
+++ b/AI_Engine/Config/formats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proyectos\Nueva carpeta\Bot-Creacion-de-Pedidos\AI_Engine\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670F138C-D8E8-471A-89EA-64FF047E1F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C521CCA7-05A4-4477-92E2-83D8C8C8E22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-130" yWindow="10690" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{CB7259FD-4C9D-4A4E-AB12-F728DAD994BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{CB7259FD-4C9D-4A4E-AB12-F728DAD994BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="139">
   <si>
     <t>client</t>
   </si>
@@ -515,6 +515,12 @@
   </si>
   <si>
     <t>[a-zA-Z]*\d{5,}</t>
+  </si>
+  <si>
+    <t>[wW] \d{1,2}\.\d{3,4}</t>
+  </si>
+  <si>
+    <t>[wW] \d{1,2}\.\d{2}</t>
   </si>
 </sst>
 </file>
@@ -1711,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA94B6A-80FD-4C88-8BB5-B4942723B82A}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2290,7 +2296,7 @@
         <v>134</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>118</v>
@@ -2307,7 +2313,7 @@
         <v>134</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
Formato de fecha D dd.mm.yyyy desagrupado y arreglo formato W ww.yyyy, cambiado metodo ocr de 70017078
</commit_message>
<xml_diff>
--- a/AI_Engine/Config/formats.xlsx
+++ b/AI_Engine/Config/formats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8DE5P2\OneDrive-Deere&amp;Co\OneDrive - Deere &amp; Co\Desktop\Proyectos\Nueva carpeta\Bot-Creacion-de-Pedidos\AI_Engine\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C521CCA7-05A4-4477-92E2-83D8C8C8E22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9895481D-600B-4B64-81F8-961A0EE2D760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{CB7259FD-4C9D-4A4E-AB12-F728DAD994BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CB7259FD-4C9D-4A4E-AB12-F728DAD994BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="147">
   <si>
     <t>client</t>
   </si>
@@ -469,21 +469,6 @@
     <t>1,234.10</t>
   </si>
   <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\d\.]+(,\d*){0,1}</t>
-    </r>
-  </si>
-  <si>
     <t>[\d,]+(\.\d*){0,1}</t>
   </si>
   <si>
@@ -508,9 +493,6 @@
     <t>%B %d, %y</t>
   </si>
   <si>
-    <t>D 31.12.2012</t>
-  </si>
-  <si>
     <t>[a-zA-Z]+\d{4,}</t>
   </si>
   <si>
@@ -521,6 +503,36 @@
   </si>
   <si>
     <t>[wW] \d{1,2}\.\d{2}</t>
+  </si>
+  <si>
+    <t>[\d\.]+(,\d*){0,1}</t>
+  </si>
+  <si>
+    <t>W %W.%Y</t>
+  </si>
+  <si>
+    <t>W %W.%y</t>
+  </si>
+  <si>
+    <t>Añadir "Monday" al text input y "%A" al format code para que coja el primer día de la semana</t>
+  </si>
+  <si>
+    <t>M mm.yyyy</t>
+  </si>
+  <si>
+    <t>Y yyyy</t>
+  </si>
+  <si>
+    <t>W ww.yyyy</t>
+  </si>
+  <si>
+    <t>M 12.2012</t>
+  </si>
+  <si>
+    <t>Y 2012</t>
+  </si>
+  <si>
+    <t>W 52.2012</t>
   </si>
 </sst>
 </file>
@@ -1675,19 +1687,19 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="E40" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F40" s="3"/>
     </row>
@@ -1696,10 +1708,10 @@
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F41" s="3"/>
     </row>
@@ -1717,8 +1729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA94B6A-80FD-4C88-8BB5-B4942723B82A}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2230,10 +2242,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>113</v>
@@ -2245,10 +2257,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>114</v>
@@ -2260,10 +2272,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>108</v>
@@ -2275,10 +2287,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>107</v>
@@ -2290,65 +2302,65 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="C40" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E40" s="3"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="C41" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E41" s="3"/>
     </row>
@@ -2368,7 +2380,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2398,7 +2410,7 @@
         <v>123</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2409,7 +2421,7 @@
         <v>124</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2429,7 +2441,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2445,7 +2457,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2462,12 +2474,12 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="1" customWidth="1"/>
     <col min="2" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -2478,7 +2490,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Añadido metodo ocr multiple
</commit_message>
<xml_diff>
--- a/AI_Engine/Config/formats.xlsx
+++ b/AI_Engine/Config/formats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deere-my.sharepoint.com/personal/gonzalezdiazsergio_johndeere_com/Documents/Desktop/Proyectos/Nueva carpeta/Bot-Creacion-de-Pedidos/AI_Engine/Config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deere-my.sharepoint.com/personal/gonzalezdiazsergio_johndeere_com/Documents/Desktop/Proyectos/Bot-Creacion-de-Pedidos/AI_Engine/Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{9895481D-600B-4B64-81F8-961A0EE2D760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B952D462-363C-44F6-AA4F-CB3ACC9EB18F}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{9895481D-600B-4B64-81F8-961A0EE2D760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09677CB4-9A90-46E3-885A-0A08ED2683D3}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11325" activeTab="2" xr2:uid="{CB7259FD-4C9D-4A4E-AB12-F728DAD994BD}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" activeTab="2" xr2:uid="{CB7259FD-4C9D-4A4E-AB12-F728DAD994BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'date (2)'!$A$1:$F$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">date_format!$A$1:$E$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">date_format!$A$1:$E$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="153">
   <si>
     <t>client</t>
   </si>
@@ -499,12 +499,6 @@
     <t>[a-zA-Z]*\d{5,}</t>
   </si>
   <si>
-    <t>[wW] \d{1,2}\.\d{3,4}</t>
-  </si>
-  <si>
-    <t>[wW] \d{1,2}\.\d{2}</t>
-  </si>
-  <si>
     <t>[\d\.]+(,\d*){0,1}</t>
   </si>
   <si>
@@ -545,6 +539,18 @@
   </si>
   <si>
     <t>M %m.%y</t>
+  </si>
+  <si>
+    <t>w \d{1,2}\.\d{3,4}</t>
+  </si>
+  <si>
+    <t>w \d{1,2}\.\d{2}</t>
+  </si>
+  <si>
+    <t>w %W.%Y</t>
+  </si>
+  <si>
+    <t>w %W.%y</t>
   </si>
 </sst>
 </file>
@@ -1739,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA94B6A-80FD-4C88-8BB5-B4942723B82A}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,7 +2239,7 @@
         <v>103</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E32" s="3"/>
     </row>
@@ -2248,46 +2254,46 @@
         <v>104</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>114</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>108</v>
@@ -2299,10 +2305,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>107</v>
@@ -2314,70 +2320,104 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="D38" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E40" s="3"/>
+        <v>137</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C42" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E41" s="3"/>
+      <c r="E43" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E39" xr:uid="{7FA94B6A-80FD-4C88-8BB5-B4942723B82A}"/>
+  <autoFilter ref="A1:E40" xr:uid="{7FA94B6A-80FD-4C88-8BB5-B4942723B82A}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
@@ -2422,7 +2462,7 @@
         <v>123</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Añadido JD Israel, arreglado error formato de fecha
</commit_message>
<xml_diff>
--- a/AI_Engine/Config/formats.xlsx
+++ b/AI_Engine/Config/formats.xlsx
@@ -1,28 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deere-my.sharepoint.com/personal/gonzalezdiazsergio_johndeere_com/Documents/Desktop/Proyectos/Bot-Creacion-de-Pedidos/AI_Engine/Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{9895481D-600B-4B64-81F8-961A0EE2D760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09677CB4-9A90-46E3-885A-0A08ED2683D3}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{9895481D-600B-4B64-81F8-961A0EE2D760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5F972E3-0C18-42F7-A09D-C87D07AA87C9}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" activeTab="2" xr2:uid="{CB7259FD-4C9D-4A4E-AB12-F728DAD994BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{CB7259FD-4C9D-4A4E-AB12-F728DAD994BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="date (2)" sheetId="5" r:id="rId2"/>
-    <sheet name="date_format" sheetId="2" r:id="rId3"/>
-    <sheet name="number_format" sheetId="3" r:id="rId4"/>
-    <sheet name="reference_format" sheetId="4" r:id="rId5"/>
-    <sheet name="order_number_format" sheetId="6" r:id="rId6"/>
+    <sheet name="date_format" sheetId="2" r:id="rId2"/>
+    <sheet name="number_format" sheetId="3" r:id="rId3"/>
+    <sheet name="reference_format" sheetId="4" r:id="rId4"/>
+    <sheet name="order_number_format" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'date (2)'!$A$1:$F$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">date_format!$A$1:$E$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">date_format!$A$1:$E$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="134">
   <si>
     <t>client</t>
   </si>
@@ -133,69 +131,6 @@
     <t>12/31/2012</t>
   </si>
   <si>
-    <t>regex_n</t>
-  </si>
-  <si>
-    <r>
-      <t>\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>d{2,4}/\d{1,2}/\d{1,2}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>d{2,4}\.\d{1,2}\.\d{1,2}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>d{2,4}\-\d{1,2}\-\d{1,2}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[a-zA-Z]{3}[ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>\-]\d{2,4}</t>
-    </r>
-  </si>
-  <si>
     <t>\d{1,2}/\d{1,2}/\d{3,4}</t>
   </si>
   <si>
@@ -208,9 +143,6 @@
     <t>%m/%d/%Y</t>
   </si>
   <si>
-    <t>\d{1,2}/\d{1,2}/\d{2,4}</t>
-  </si>
-  <si>
     <t>%m/%d/%y</t>
   </si>
   <si>
@@ -250,9 +182,6 @@
     <t>%y/%d/%m</t>
   </si>
   <si>
-    <t>\d{1,2}\.\d{1,2}\.\d{2,4}</t>
-  </si>
-  <si>
     <t>\d{1,2}\.\d{1,2}\.\d{3,4}</t>
   </si>
   <si>
@@ -298,9 +227,6 @@
     <t>2012.31.12</t>
   </si>
   <si>
-    <t>\d{1,2}\-\d{1,2}\-\d{2,4}</t>
-  </si>
-  <si>
     <t>%d-%m-%Y</t>
   </si>
   <si>
@@ -349,9 +275,6 @@
     <t>December-2012</t>
   </si>
   <si>
-    <t>[a-zA-Z]{3,9}[ \-]\d{2,4}</t>
-  </si>
-  <si>
     <t>%B-%Y</t>
   </si>
   <si>
@@ -370,9 +293,6 @@
     <t>dd Month yyyy</t>
   </si>
   <si>
-    <t>\d{1,2} [a-zA-Z]{3} \d{2,4}</t>
-  </si>
-  <si>
     <t>ShortMonth-yyyy</t>
   </si>
   <si>
@@ -409,12 +329,6 @@
     <t>D \d{1,2}\.\d{1,2}\.\d{2}</t>
   </si>
   <si>
-    <t>D %d %m %Y</t>
-  </si>
-  <si>
-    <t>D %d %m %y</t>
-  </si>
-  <si>
     <t>Y \d{2}</t>
   </si>
   <si>
@@ -439,27 +353,9 @@
     <t>M \d{1,2}\.\d{2}</t>
   </si>
   <si>
-    <t>M %m %Y</t>
-  </si>
-  <si>
-    <t>M %m %y</t>
-  </si>
-  <si>
-    <t>[DMYW] (\d{1,2}\.)?(\d{1,2}\.)?\d{2,4}</t>
-  </si>
-  <si>
-    <t>W %W %Y %d</t>
-  </si>
-  <si>
-    <t>W %W %y %d</t>
-  </si>
-  <si>
     <t>needs_processing</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>example</t>
   </si>
   <si>
@@ -476,9 +372,6 @@
   </si>
   <si>
     <t>December 31, 2012</t>
-  </si>
-  <si>
-    <t>[a-zA-Z]+ \d{1,2}, *\d{2,4}</t>
   </si>
   <si>
     <t>[a-zA-Z]+ \d{1,2}, *\d{3,4}</t>
@@ -1109,646 +1002,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE714AAC-4807-4497-8078-EB461928AC64}">
-  <dimension ref="A1:F41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F41" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:F39" xr:uid="{7FA94B6A-80FD-4C88-8BB5-B4942723B82A}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;R&amp;1#&amp;"Calibri"&amp;10&amp;KFF0000Company Use</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA94B6A-80FD-4C88-8BB5-B4942723B82A}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1766,7 +1024,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>14</v>
@@ -1775,7 +1033,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1786,7 +1044,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>17</v>
@@ -1801,10 +1059,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -1816,10 +1074,10 @@
         <v>28</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -1831,10 +1089,10 @@
         <v>28</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E5" s="3"/>
     </row>
@@ -1843,13 +1101,13 @@
         <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -1858,13 +1116,13 @@
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -1873,13 +1131,13 @@
         <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E8" s="3"/>
     </row>
@@ -1888,13 +1146,13 @@
         <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E9" s="3"/>
     </row>
@@ -1903,13 +1161,13 @@
         <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -1918,13 +1176,13 @@
         <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -1933,13 +1191,13 @@
         <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -1948,13 +1206,13 @@
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -1963,13 +1221,13 @@
         <v>22</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -1978,13 +1236,13 @@
         <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E15" s="3"/>
     </row>
@@ -1993,13 +1251,13 @@
         <v>23</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E16" s="3"/>
     </row>
@@ -2008,13 +1266,13 @@
         <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -2023,13 +1281,13 @@
         <v>24</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E18" s="3"/>
     </row>
@@ -2038,13 +1296,13 @@
         <v>24</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E19" s="3"/>
     </row>
@@ -2053,13 +1311,13 @@
         <v>25</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E20" s="3"/>
     </row>
@@ -2068,13 +1326,13 @@
         <v>25</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E21" s="3"/>
     </row>
@@ -2083,13 +1341,13 @@
         <v>26</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E22" s="3"/>
     </row>
@@ -2098,13 +1356,13 @@
         <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E23" s="3"/>
     </row>
@@ -2113,13 +1371,13 @@
         <v>27</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E24" s="3"/>
     </row>
@@ -2128,291 +1386,291 @@
         <v>27</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="E43" s="3"/>
     </row>
@@ -2427,7 +1685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A1F479-548D-44CD-974F-81D5E9B1FF5A}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2448,7 +1706,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>14</v>
@@ -2459,10 +1717,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2470,10 +1728,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2488,7 +1746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A813717D-269B-401B-BF68-058F01D045C7}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2509,7 +1767,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2521,7 +1779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DA351C-3B7F-4084-B19B-EF412F91127A}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -2542,7 +1800,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>